<commit_message>
add brand logo, update products description
</commit_message>
<xml_diff>
--- a/src/assets/Productos.xlsx
+++ b/src/assets/Productos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Google Drive\Nico\Programacion\CoderHouse\React\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Google Drive\Nico\Programacion\CoderHouse\React\lorences-proyecto-react\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BC7F16-E7F5-4F56-9470-F5F4DCA202C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50392719-6E7B-4167-8F52-55581D54F6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$29</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="84">
   <si>
     <t>id</t>
   </si>
@@ -98,12 +98,6 @@
     <t>Jaque Mate Cabernet Franc Reserva</t>
   </si>
   <si>
-    <t>Dinastia Extra Brut</t>
-  </si>
-  <si>
-    <t>Siete Vacas Espumante Origen</t>
-  </si>
-  <si>
     <t>Las Perdices Exploracion Casablanca</t>
   </si>
   <si>
@@ -155,9 +149,6 @@
     <t>https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/b70f29_8e4dad2d25ce4bd095bec3526c879622_mv21-894e6a192cca6be4a916140947136105-640-0.jpg</t>
   </si>
   <si>
-    <t>Aristides Icono Extra Brut</t>
-  </si>
-  <si>
     <t>https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/mythic-petit1-30efff58dec427067d16020749360771-640-0.jpg</t>
   </si>
   <si>
@@ -173,9 +164,6 @@
     <t>https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/jaque-mate-reserva-cabernet-franc1-d18095e7ea9904ec1215986530742040-640-0.jpg</t>
   </si>
   <si>
-    <t>https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/dinastia-extra-brut1-fde1971258837dfc8615936465803748-640-0.jpg</t>
-  </si>
-  <si>
     <t>https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/vino-las-perdices-exploracion-casa-blanca-sauvignon-blanc-d_nq_np_693115-mla29480640575_022019-f1-632ae12afe7abda88f15902635029767-640-0.jpg</t>
   </si>
   <si>
@@ -243,6 +231,63 @@
   </si>
   <si>
     <t>cervezas</t>
+  </si>
+  <si>
+    <t>bodega</t>
+  </si>
+  <si>
+    <t>De color rojo rubí intenso con bordes violáceos. En nariz es muy frutado típico de la región, con notas de ciruelas, pasas de uva y pimienta. En boca es voluminoso, de estructura intensa, con taninos suaves y amables, final equilibrado y armónico.</t>
+  </si>
+  <si>
+    <t>De color rojo rubí intenso con bordes violáceos. En nariz es frutado y típico con notas de pimiento, pimienta y especies. En boca es de buen volumen y estructura armónica, con buen final de taninos suaves y maduros</t>
+  </si>
+  <si>
+    <t>De color rojo rubí intenso con borde violáceos. En nariz es frutado y típico con notas de pimiento,  pimienta y especies. En boca tiene buen volumen y estructura armónica, con buen final de taninos suaves y maduros.</t>
+  </si>
+  <si>
+    <t>De color rojo morado rubí, tirando a granate. En nariz es frutado y típico con notas de pimientos asado, pimienta, especies y delicado sabor a frutos negros maduros. En boca es de buen volumen y estructura, armónica con buen final de taninos intensos y maduros.</t>
+  </si>
+  <si>
+    <t>Siete Vacas Espumante Rosado</t>
+  </si>
+  <si>
+    <t>Aristides Confidencial Extra Brut</t>
+  </si>
+  <si>
+    <t>Bodega Las Arcas de Tolombon - Valle Calchaquí</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bodega Aristides </t>
+  </si>
+  <si>
+    <t>Bodega Enrique Foster – Luján de Cuyo</t>
+  </si>
+  <si>
+    <t>Mythic Wine - Mendoza</t>
+  </si>
+  <si>
+    <t>Bodegas y Viñedos Sánchez</t>
+  </si>
+  <si>
+    <t>Viña Las Perdices</t>
+  </si>
+  <si>
+    <t>Huarpe Wines - Agrelo, Lujan de Cuyo</t>
+  </si>
+  <si>
+    <t>Bodega DiamAndes</t>
+  </si>
+  <si>
+    <t>Bodega Cruzat - Mendoza</t>
+  </si>
+  <si>
+    <t>Bodega Kaiken</t>
+  </si>
+  <si>
+    <t>De color amarillo claro con tonalidades verdosas, límpido y brillante. En nariz es muy frutado, típico de la región, con sutiles notas de durazno blanco y cítricos. En boca es amable, fresco, con final largo y equilibrado</t>
+  </si>
+  <si>
+    <t>Espumante Blanc de Noir, elaborado con uvas Malbec con el método Charmat lungo. En la copa, las burbujas son pequeñas y firmes. En la nariz encontramos aromas frutados típicos de la variedad, como guinda y cereza; junto como leves notas a panificados. En la boca es suave, con una excelente acidez y buen cuerpo. La burbuja destaca la frescura por su persistencia.</t>
   </si>
 </sst>
 </file>
@@ -562,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28:F30"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,13 +618,14 @@
     <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.44140625" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" customWidth="1"/>
+    <col min="5" max="5" width="33.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -590,19 +636,22 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -612,21 +661,27 @@
       <c r="C2">
         <v>900</v>
       </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2">
-        <v>10</v>
-      </c>
-      <c r="I2" t="str">
-        <f>+CONCATENATE("{id:",A2,", title: '",B2,"', price: ",C2,", description: '",D2,"', pictureUrl: '",E2,"', category: '",F2,"', stock: ",G2,"},")</f>
-        <v>{id:1, title: 'Siete Vacas Torrontes', price: 900, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/siete-vacas-torrontes1-99271abbb27498181f16032285125101-640-0.jpg', category: 'blancos', stock: 10},</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+      <c r="G2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="J2" t="str">
+        <f>+CONCATENATE("{id:",A2,", title: '",B2,"', price: ",C2,", bodega: '",D2,"', description: '",E2,"', pictureUrl: '",F2,"', category: '",G2,"', stock: ",H2,"},")</f>
+        <v>{id:1, title: 'Siete Vacas Torrontes', price: 900, bodega: 'Bodega Las Arcas de Tolombon - Valle Calchaquí', description: 'De color amarillo claro con tonalidades verdosas, límpido y brillante. En nariz es muy frutado, típico de la región, con sutiles notas de durazno blanco y cítricos. En boca es amable, fresco, con final largo y equilibrado', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/siete-vacas-torrontes1-99271abbb27498181f16032285125101-640-0.jpg', category: 'blancos', stock: 10},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>+A2+1</f>
         <v>2</v>
@@ -637,23 +692,29 @@
       <c r="C3">
         <v>900</v>
       </c>
+      <c r="D3" t="s">
+        <v>72</v>
+      </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3">
-        <v>10</v>
-      </c>
-      <c r="I3" t="str">
-        <f t="shared" ref="I3:I30" si="0">+CONCATENATE("{id:",A3,", title: '",B3,"', price: ",C3,", description: '",D3,"', pictureUrl: '",E3,"', category: '",F3,"', stock: ",G3,"},")</f>
-        <v>{id:2, title: 'Siete Vacas Malbec Origen', price: 900, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/siete-vacas-malbec1-a373d43bd398896c8516032280594428-640-0.jpg', category: 'tintos', stock: 10},</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="G3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J29" si="0">+CONCATENATE("{id:",A3,", title: '",B3,"', price: ",C3,", bodega: '",D3,"', description: '",E3,"', pictureUrl: '",F3,"', category: '",G3,"', stock: ",H3,"},")</f>
+        <v>{id:2, title: 'Siete Vacas Malbec Origen', price: 900, bodega: 'Bodega Las Arcas de Tolombon - Valle Calchaquí', description: 'De color rojo rubí intenso con bordes violáceos. En nariz es muy frutado típico de la región, con notas de ciruelas, pasas de uva y pimienta. En boca es voluminoso, de estructura intensa, con taninos suaves y amables, final equilibrado y armónico.', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/siete-vacas-malbec1-a373d43bd398896c8516032280594428-640-0.jpg', category: 'tintos', stock: 10},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f t="shared" ref="A4:A30" si="1">+A3+1</f>
+        <f t="shared" ref="A4:A29" si="1">+A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -662,46 +723,58 @@
       <c r="C4">
         <v>900</v>
       </c>
+      <c r="D4" t="s">
+        <v>72</v>
+      </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F4" t="s">
         <v>59</v>
       </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
-      <c r="I4" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:3, title: 'Siete Vacas Cabernet Sauvignon Origen', price: 900, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/siete-vacas-cabernet-sauvignon1-01a1671e17067e49ed16032278974733-640-0.jpg', category: 'tintos', stock: 10},</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:3, title: 'Siete Vacas Cabernet Sauvignon Origen', price: 900, bodega: 'Bodega Las Arcas de Tolombon - Valle Calchaquí', description: 'De color rojo rubí intenso con bordes violáceos. En nariz es frutado y típico con notas de pimiento, pimienta y especies. En boca es de buen volumen y estructura armónica, con buen final de taninos suaves y maduros', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/siete-vacas-cabernet-sauvignon1-01a1671e17067e49ed16032278974733-640-0.jpg', category: 'tintos', stock: 10},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C5">
         <v>1550</v>
       </c>
+      <c r="D5" t="s">
+        <v>72</v>
+      </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G5">
-        <v>10</v>
-      </c>
-      <c r="I5" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:4, title: 'Siete Vacas Cabernet Sauvignon Reserva', price: 1550, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/siete-vacas-reserva-cabernet-sauvignon1-4c110db567cf9dbb6716032275610969-640-0.jpg', category: 'tintos', stock: 10},</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+      <c r="G5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:4, title: 'Siete Vacas Cabernet Sauvignon Reserva', price: 1550, bodega: 'Bodega Las Arcas de Tolombon - Valle Calchaquí', description: 'De color rojo rubí intenso con borde violáceos. En nariz es frutado y típico con notas de pimiento,  pimienta y especies. En boca tiene buen volumen y estructura armónica, con buen final de taninos suaves y maduros.', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/siete-vacas-reserva-cabernet-sauvignon1-4c110db567cf9dbb6716032275610969-640-0.jpg', category: 'tintos', stock: 10},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -712,71 +785,86 @@
       <c r="C6">
         <v>1550</v>
       </c>
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="F6" t="s">
-        <v>59</v>
-      </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
-      <c r="I6" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:5, title: 'Siete Vacas Tannat Reserva', price: 1550, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/siete-vacas-reserva-tannat1-72b783d84f338815e116032270632961-640-0.jpg', category: 'tintos', stock: 10},</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="G6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6">
+        <v>10</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:5, title: 'Siete Vacas Tannat Reserva', price: 1550, bodega: 'Bodega Las Arcas de Tolombon - Valle Calchaquí', description: 'De color rojo morado rubí, tirando a granate. En nariz es frutado y típico con notas de pimientos asado, pimienta, especies y delicado sabor a frutos negros maduros. En boca es de buen volumen y estructura, armónica con buen final de taninos intensos y maduros.', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/siete-vacas-reserva-tannat1-72b783d84f338815e116032270632961-640-0.jpg', category: 'tintos', stock: 10},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="C7">
-        <v>925</v>
+        <v>1300</v>
+      </c>
+      <c r="D7" t="s">
+        <v>74</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="F7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G7">
-        <v>10</v>
-      </c>
-      <c r="I7" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:6, title: 'Siete Vacas Espumante Origen', price: 925, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/siete-vacas-espumante1-d84dfd95608371867016032268477868-640-0.jpg', category: 'espumantes', stock: 10},</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="G7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:6, title: 'Siete Vacas Espumante Rosado', price: 1300, bodega: 'Bodega Enrique Foster – Luján de Cuyo', description: 'Espumante Blanc de Noir, elaborado con uvas Malbec con el método Charmat lungo. En la copa, las burbujas son pequeñas y firmes. En la nariz encontramos aromas frutados típicos de la variedad, como guinda y cereza; junto como leves notas a panificados. En la boca es suave, con una excelente acidez y buen cuerpo. La burbuja destaca la frescura por su persistencia.', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/siete-vacas-espumante1-d84dfd95608371867016032268477868-640-0.jpg', category: 'espumantes', stock: 10},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="C8">
         <v>2415</v>
       </c>
-      <c r="E8" t="s">
-        <v>38</v>
+      <c r="D8" t="s">
+        <v>73</v>
       </c>
       <c r="F8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8">
-        <v>10</v>
-      </c>
-      <c r="I8" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:7, title: 'Aristides Icono Extra Brut', price: 2415, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/b70f29_8e4dad2d25ce4bd095bec3526c879622_mv21-894e6a192cca6be4a916140947136105-640-0.jpg', category: 'espumantes', stock: 10},</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:7, title: 'Aristides Confidencial Extra Brut', price: 2415, bodega: 'Bodega Aristides ', description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/b70f29_8e4dad2d25ce4bd095bec3526c879622_mv21-894e6a192cca6be4a916140947136105-640-0.jpg', category: 'espumantes', stock: 10},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -787,21 +875,24 @@
       <c r="C9">
         <v>770</v>
       </c>
-      <c r="E9" t="s">
-        <v>34</v>
+      <c r="D9" t="s">
+        <v>73</v>
       </c>
       <c r="F9" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9">
-        <v>10</v>
-      </c>
-      <c r="I9" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:8, title: 'Aristides Bonarda', price: 770, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/aristides_bonarda1-c41bf24591115a66a115131748388183-640-0.gif', category: 'tintos', stock: 10},</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="G9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:8, title: 'Aristides Bonarda', price: 770, bodega: 'Bodega Aristides ', description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/aristides_bonarda1-c41bf24591115a66a115131748388183-640-0.gif', category: 'tintos', stock: 10},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -812,21 +903,24 @@
       <c r="C10">
         <v>770</v>
       </c>
-      <c r="E10" t="s">
-        <v>35</v>
+      <c r="D10" t="s">
+        <v>73</v>
       </c>
       <c r="F10" t="s">
-        <v>59</v>
-      </c>
-      <c r="G10">
-        <v>10</v>
-      </c>
-      <c r="I10" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:9, title: 'Aristides Merlot', price: 770, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/aristides-merlot1-6156359b2e4b06d28015814351831121-640-0.jpg', category: 'tintos', stock: 10},</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="G10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:9, title: 'Aristides Merlot', price: 770, bodega: 'Bodega Aristides ', description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/aristides-merlot1-6156359b2e4b06d28015814351831121-640-0.jpg', category: 'tintos', stock: 10},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -837,21 +931,24 @@
       <c r="C11">
         <v>770</v>
       </c>
-      <c r="E11" t="s">
-        <v>36</v>
+      <c r="D11" t="s">
+        <v>73</v>
       </c>
       <c r="F11" t="s">
-        <v>59</v>
-      </c>
-      <c r="G11">
-        <v>10</v>
-      </c>
-      <c r="I11" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:10, title: 'Aristides Malbec', price: 770, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/aristides_malbec1-2df63744d2b6f0e3d815131748530477-640-0.gif', category: 'tintos', stock: 10},</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="G11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:10, title: 'Aristides Malbec', price: 770, bodega: 'Bodega Aristides ', description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/aristides_malbec1-2df63744d2b6f0e3d815131748530477-640-0.gif', category: 'tintos', stock: 10},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -862,21 +959,24 @@
       <c r="C12">
         <v>770</v>
       </c>
-      <c r="E12" t="s">
-        <v>37</v>
+      <c r="D12" t="s">
+        <v>73</v>
       </c>
       <c r="F12" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12">
-        <v>10</v>
-      </c>
-      <c r="I12" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:11, title: 'Aristides Cabernet Sauvignon', price: 770, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/aristides_cabernet1-9bfeefd99e1bfc153d15131748461602-640-0.gif', category: 'tintos', stock: 10},</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="G12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:11, title: 'Aristides Cabernet Sauvignon', price: 770, bodega: 'Bodega Aristides ', description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/aristides_cabernet1-9bfeefd99e1bfc153d15131748461602-640-0.gif', category: 'tintos', stock: 10},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -887,21 +987,24 @@
       <c r="C13">
         <v>990</v>
       </c>
-      <c r="E13" t="s">
-        <v>42</v>
+      <c r="D13" t="s">
+        <v>75</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
-      </c>
-      <c r="G13">
-        <v>10</v>
-      </c>
-      <c r="I13" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:12, title: 'Mythic Mountain Cabernet Franc', price: 990, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/mythic-cabernet-franc1-3b27f9d76d4a0eac9716020753480970-640-0.jpg', category: 'tintos', stock: 10},</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="G13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13">
+        <v>10</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:12, title: 'Mythic Mountain Cabernet Franc', price: 990, bodega: 'Mythic Wine - Mendoza', description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/mythic-cabernet-franc1-3b27f9d76d4a0eac9716020753480970-640-0.jpg', category: 'tintos', stock: 10},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -912,21 +1015,24 @@
       <c r="C14">
         <v>990</v>
       </c>
-      <c r="E14" t="s">
-        <v>40</v>
+      <c r="D14" t="s">
+        <v>75</v>
       </c>
       <c r="F14" t="s">
-        <v>59</v>
-      </c>
-      <c r="G14">
-        <v>10</v>
-      </c>
-      <c r="I14" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:13, title: 'Mythic Mountain Petit Verdot', price: 990, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/mythic-petit1-30efff58dec427067d16020749360771-640-0.jpg', category: 'tintos', stock: 10},</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="G14" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14">
+        <v>10</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:13, title: 'Mythic Mountain Petit Verdot', price: 990, bodega: 'Mythic Wine - Mendoza', description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/mythic-petit1-30efff58dec427067d16020749360771-640-0.jpg', category: 'tintos', stock: 10},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -937,21 +1043,24 @@
       <c r="C15">
         <v>1390</v>
       </c>
-      <c r="E15" t="s">
-        <v>41</v>
+      <c r="D15" t="s">
+        <v>75</v>
       </c>
       <c r="F15" t="s">
-        <v>58</v>
-      </c>
-      <c r="G15">
-        <v>10</v>
-      </c>
-      <c r="I15" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:14, title: 'Mythic Vineyard Blanc de Blanc', price: 1390, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/mythic-blanc-de-blancs1-26bc333f3ee0cef08c15985024394047-1024-10241-ca095d7760423d68b716020717181137-640-0.png', category: 'blancos', stock: 10},</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="G15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15">
+        <v>10</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:14, title: 'Mythic Vineyard Blanc de Blanc', price: 1390, bodega: 'Mythic Wine - Mendoza', description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/mythic-blanc-de-blancs1-26bc333f3ee0cef08c15985024394047-1024-10241-ca095d7760423d68b716020717181137-640-0.png', category: 'blancos', stock: 10},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -962,21 +1071,24 @@
       <c r="C16">
         <v>740</v>
       </c>
-      <c r="E16" t="s">
-        <v>43</v>
+      <c r="D16" t="s">
+        <v>76</v>
       </c>
       <c r="F16" t="s">
-        <v>58</v>
-      </c>
-      <c r="G16">
-        <v>10</v>
-      </c>
-      <c r="I16" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:15, title: 'Jaque Mate Sauvignon Blanc', price: 740, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/jaque-mate-sauvignon-blanc1-d93bb26d687b00643515986539494118-640-0.jpg', category: 'blancos', stock: 10},</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="G16" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16">
+        <v>10</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:15, title: 'Jaque Mate Sauvignon Blanc', price: 740, bodega: 'Bodegas y Viñedos Sánchez', description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/jaque-mate-sauvignon-blanc1-d93bb26d687b00643515986539494118-640-0.jpg', category: 'blancos', stock: 10},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -987,21 +1099,24 @@
       <c r="C17">
         <v>1115</v>
       </c>
-      <c r="E17" t="s">
-        <v>44</v>
+      <c r="D17" t="s">
+        <v>76</v>
       </c>
       <c r="F17" t="s">
-        <v>59</v>
-      </c>
-      <c r="G17">
-        <v>10</v>
-      </c>
-      <c r="I17" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:16, title: 'Jaque Mate Cabernet Franc Reserva', price: 1115, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/jaque-mate-reserva-cabernet-franc1-d18095e7ea9904ec1215986530742040-640-0.jpg', category: 'tintos', stock: 10},</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="G17" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17">
+        <v>10</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:16, title: 'Jaque Mate Cabernet Franc Reserva', price: 1115, bodega: 'Bodegas y Viñedos Sánchez', description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/jaque-mate-reserva-cabernet-franc1-d18095e7ea9904ec1215986530742040-640-0.jpg', category: 'tintos', stock: 10},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -1010,123 +1125,138 @@
         <v>20</v>
       </c>
       <c r="C18">
-        <v>920</v>
-      </c>
-      <c r="E18" t="s">
-        <v>45</v>
+        <v>2150</v>
+      </c>
+      <c r="D18" t="s">
+        <v>77</v>
       </c>
       <c r="F18" t="s">
-        <v>60</v>
-      </c>
-      <c r="G18">
-        <v>10</v>
-      </c>
-      <c r="I18" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:17, title: 'Dinastia Extra Brut', price: 920, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/dinastia-extra-brut1-fde1971258837dfc8615936465803748-640-0.jpg', category: 'espumantes', stock: 10},</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="G18" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18">
+        <v>10</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:17, title: 'Las Perdices Exploracion Casablanca', price: 2150, bodega: 'Viña Las Perdices', description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/vino-las-perdices-exploracion-casa-blanca-sauvignon-blanc-d_nq_np_693115-mla29480640575_022019-f1-632ae12afe7abda88f15902635029767-640-0.jpg', category: 'blancos', stock: 10},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19">
-        <v>2150</v>
-      </c>
-      <c r="E19" t="s">
+        <v>770</v>
+      </c>
+      <c r="D19" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" t="s">
         <v>46</v>
       </c>
-      <c r="F19" t="s">
-        <v>58</v>
-      </c>
-      <c r="G19">
-        <v>10</v>
-      </c>
-      <c r="I19" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:18, title: 'Las Perdices Exploracion Casablanca', price: 2150, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/vino-las-perdices-exploracion-casa-blanca-sauvignon-blanc-d_nq_np_693115-mla29480640575_022019-f1-632ae12afe7abda88f15902635029767-640-0.jpg', category: 'blancos', stock: 10},</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G19" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19">
+        <v>10</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:18, title: 'Taymente Cabernet Sauvignon', price: 770, bodega: 'Huarpe Wines - Agrelo, Lujan de Cuyo', description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/taymente-cabernet1-0d1d54ddb79bc65c1a15901965389939-640-0.jpg', category: 'tintos', stock: 10},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C20">
         <v>770</v>
       </c>
-      <c r="E20" t="s">
-        <v>50</v>
+      <c r="D20" t="s">
+        <v>78</v>
       </c>
       <c r="F20" t="s">
-        <v>59</v>
-      </c>
-      <c r="G20">
-        <v>10</v>
-      </c>
-      <c r="I20" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:19, title: 'Taymente Cabernet Sauvignon', price: 770, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/taymente-cabernet1-0d1d54ddb79bc65c1a15901965389939-640-0.jpg', category: 'tintos', stock: 10},</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="G20" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20">
+        <v>10</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:19, title: 'Taymente Malbec', price: 770, bodega: 'Huarpe Wines - Agrelo, Lujan de Cuyo', description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/taymentes-malbec1-c3ed51ba8509bf29bf15901956387642-640-0.jpg', category: 'tintos', stock: 10},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C21">
-        <v>770</v>
-      </c>
-      <c r="E21" t="s">
-        <v>49</v>
+        <v>665</v>
+      </c>
+      <c r="D21" t="s">
+        <v>78</v>
       </c>
       <c r="F21" t="s">
-        <v>59</v>
-      </c>
-      <c r="G21">
-        <v>10</v>
-      </c>
-      <c r="I21" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:20, title: 'Taymente Malbec', price: 770, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/taymentes-malbec1-c3ed51ba8509bf29bf15901956387642-640-0.jpg', category: 'tintos', stock: 10},</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="G21" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21">
+        <v>10</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:20, title: 'Taymente Sauvignon Blanc', price: 665, bodega: 'Huarpe Wines - Agrelo, Lujan de Cuyo', description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/taymentesauvblanc1-ff236c04418e11694e15901960555090-640-0.jpg', category: 'blancos', stock: 10},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22">
         <v>665</v>
       </c>
-      <c r="E22" t="s">
-        <v>48</v>
+      <c r="D22" t="s">
+        <v>78</v>
       </c>
       <c r="F22" t="s">
-        <v>58</v>
-      </c>
-      <c r="G22">
-        <v>10</v>
-      </c>
-      <c r="I22" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:21, title: 'Taymente Sauvignon Blanc', price: 665, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/taymentesauvblanc1-ff236c04418e11694e15901960555090-640-0.jpg', category: 'blancos', stock: 10},</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="G22" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22">
+        <v>10</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:21, title: 'Taymente Chardonnay', price: 665, bodega: 'Huarpe Wines - Agrelo, Lujan de Cuyo', description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/taymentechardonnay1-a0f7fe3c51b863255e15901959124134-640-0.jpg', category: 'blancos', stock: 10},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -1135,98 +1265,107 @@
         <v>25</v>
       </c>
       <c r="C23">
-        <v>665</v>
-      </c>
-      <c r="E23" t="s">
+        <v>2000</v>
+      </c>
+      <c r="D23" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" t="s">
         <v>47</v>
       </c>
-      <c r="F23" t="s">
-        <v>58</v>
-      </c>
-      <c r="G23">
-        <v>10</v>
-      </c>
-      <c r="I23" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:22, title: 'Taymente Chardonnay', price: 665, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/taymentechardonnay1-a0f7fe3c51b863255e15901959124134-640-0.jpg', category: 'blancos', stock: 10},</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G23" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23">
+        <v>10</v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:22, title: 'Diamandes de Uco Viognier', price: 2000, bodega: 'Bodega DiamAndes', description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/viognier1-c63a2fac85643a734315900676282614-640-0.jpg', category: 'blancos', stock: 10},</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24">
+        <v>1750</v>
+      </c>
+      <c r="D24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F24" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" t="s">
+        <v>56</v>
+      </c>
+      <c r="H24">
+        <v>10</v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:23, title: 'Cruzat Naranjo', price: 1750, bodega: 'Bodega Cruzat - Mendoza', description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/cruzat-naranjo11-f532b1fbe21b2b64a016297282096161-640-0.png', category: 'espumantes', stock: 10},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
         <v>27</v>
       </c>
-      <c r="C24">
-        <v>2000</v>
-      </c>
-      <c r="E24" t="s">
-        <v>51</v>
-      </c>
-      <c r="F24" t="s">
-        <v>58</v>
-      </c>
-      <c r="G24">
-        <v>10</v>
-      </c>
-      <c r="I24" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:23, title: 'Diamandes de Uco Viognier', price: 2000, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/viognier1-c63a2fac85643a734315900676282614-640-0.jpg', category: 'blancos', stock: 10},</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="C25">
+        <v>1350</v>
+      </c>
+      <c r="D25" t="s">
+        <v>81</v>
+      </c>
+      <c r="F25" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" t="s">
+        <v>56</v>
+      </c>
+      <c r="H25">
+        <v>10</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:24, title: 'Kaiken Brut', price: 1350, bodega: 'Bodega Kaiken', description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/kaiken_espumante_brut-42ca00f9a8cdc9577315131761151759-480-0.gif', category: 'espumantes', stock: 10},</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
         <v>28</v>
       </c>
-      <c r="C25">
-        <v>1750</v>
-      </c>
-      <c r="E25" t="s">
-        <v>52</v>
-      </c>
-      <c r="F25" t="s">
-        <v>60</v>
-      </c>
-      <c r="G25">
-        <v>10</v>
-      </c>
-      <c r="I25" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:24, title: 'Cruzat Naranjo', price: 1750, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/cruzat-naranjo11-f532b1fbe21b2b64a016297282096161-640-0.png', category: 'espumantes', stock: 10},</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>29</v>
-      </c>
       <c r="C26">
-        <v>1350</v>
-      </c>
-      <c r="E26" t="s">
-        <v>53</v>
+        <v>365</v>
       </c>
       <c r="F26" t="s">
-        <v>60</v>
-      </c>
-      <c r="G26">
-        <v>10</v>
-      </c>
-      <c r="I26" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:25, title: 'Kaiken Brut', price: 1350, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/kaiken_espumante_brut-42ca00f9a8cdc9577315131761151759-480-0.gif', category: 'espumantes', stock: 10},</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="G26" t="s">
+        <v>64</v>
+      </c>
+      <c r="H26">
+        <v>10</v>
+      </c>
+      <c r="J26" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:25, title: 'Me Echo la Burra Triple IPA', price: 365, bodega: '', description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/me-echo-la-burra-ipa1-c963108c6257c3614f15837725038212-640-0.jpg', category: 'cervezas', stock: 10},</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -1237,46 +1376,46 @@
       <c r="C27">
         <v>365</v>
       </c>
-      <c r="E27" t="s">
-        <v>54</v>
-      </c>
       <c r="F27" t="s">
-        <v>68</v>
-      </c>
-      <c r="G27">
-        <v>10</v>
-      </c>
-      <c r="I27" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:26, title: 'Me Echo la Burra Triple IPA', price: 365, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/me-echo-la-burra-ipa1-c963108c6257c3614f15837725038212-640-0.jpg', category: 'cervezas', stock: 10},</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H27">
+        <v>10</v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:26, title: 'Me Echo la Burra Roja', price: 365, bodega: '', description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/burra-ro1-5bd69db5748a6ce73014628316097455-640-0.gif', category: 'cervezas', stock: 10},</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C28">
         <v>365</v>
       </c>
-      <c r="E28" t="s">
-        <v>57</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G28">
-        <v>10</v>
-      </c>
-      <c r="I28" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:27, title: 'Me Echo la Burra Roja', price: 365, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/burra-ro1-5bd69db5748a6ce73014628316097455-640-0.gif', category: 'cervezas', stock: 10},</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F28" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H28">
+        <v>10</v>
+      </c>
+      <c r="J28" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:27, title: 'Me Echo la Burra Rubia', price: 365, bodega: '', description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/me-echo-la-burra-rubia1-7f168d0616faa55c8516022861298126-640-0.jpg', category: 'cervezas', stock: 10},</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -1287,47 +1426,22 @@
       <c r="C29">
         <v>365</v>
       </c>
-      <c r="E29" t="s">
-        <v>56</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G29">
-        <v>10</v>
-      </c>
-      <c r="I29" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:28, title: 'Me Echo la Burra Rubia', price: 365, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/me-echo-la-burra-rubia1-7f168d0616faa55c8516022861298126-640-0.jpg', category: 'cervezas', stock: 10},</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <f t="shared" si="1"/>
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30">
-        <v>365</v>
-      </c>
-      <c r="E30" t="s">
-        <v>55</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G30">
-        <v>10</v>
-      </c>
-      <c r="I30" t="str">
-        <f t="shared" si="0"/>
-        <v>{id:29, title: 'Me Echo la Burra Negra', price: 365, description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/burra-n11-682ba221630852f18614628309249835-640-0.gif', category: 'cervezas', stock: 10},</v>
+      <c r="F29" t="s">
+        <v>51</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H29">
+        <v>10</v>
+      </c>
+      <c r="J29" t="str">
+        <f t="shared" si="0"/>
+        <v>{id:28, title: 'Me Echo la Burra Negra', price: 365, bodega: '', description: '', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/burra-n11-682ba221630852f18614628309249835-640-0.gif', category: 'cervezas', stock: 10},</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I30" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:J29" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
add ItemCount on ItemList
</commit_message>
<xml_diff>
--- a/src/assets/Productos.xlsx
+++ b/src/assets/Productos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Google Drive\Nico\Programacion\CoderHouse\React\lorences-proyecto-react\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E6F78B-9265-48B2-97E4-070F30B094A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22C201C-A41F-449A-9496-FDA800003792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="106">
   <si>
     <t>id</t>
   </si>
@@ -354,6 +354,9 @@
   </si>
   <si>
     <t>De espuma cremosa y densa de color beige. En nariz desarrolla un toque de  caramelo y mermelada de damasco.  La primera boca  da un sabor dulce y frutal, después viene el amargo caramelizado. Presenta una linda fusión de las malta y de regusto de lúpulus con sus suaves amargos.</t>
+  </si>
+  <si>
+    <t>Color verde tenue. Aromas a ruda, espárrago, hojas de tomate, con notas minerales propias de esta región. En boca, buen ataque, sabor intenso, acidez bien presente remarcando las notas de espárrago. Ideal como aperitivo o para acompañar mariscos, ostras y frutos de frutos de mar en general.</t>
   </si>
 </sst>
 </file>
@@ -362,7 +365,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="0.000000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -406,7 +409,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -691,7 +694,7 @@
   <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G57" sqref="D33:G57"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -736,7 +739,7 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C2">
@@ -767,7 +770,7 @@
         <f>+A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C3">
@@ -798,7 +801,7 @@
         <f t="shared" ref="A4:A26" si="1">+A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C4">
@@ -829,7 +832,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C5">
@@ -860,7 +863,7 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C6">
@@ -891,7 +894,7 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C7">
@@ -922,7 +925,7 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C8">
@@ -1149,7 +1152,7 @@
         <v>75</v>
       </c>
       <c r="E15" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="F15" t="s">
         <v>41</v>
@@ -1162,8 +1165,7 @@
       </c>
       <c r="J15" t="str">
         <f t="shared" si="0"/>
-        <v>{title: 'Las Perdices Exploracion Casablanca', price: 2150, bodega: 'Viña Las Perdices', description: 'Color verde tenue. Aromas a ruda, espárrago, hojas de tomate, con notas minerales propias de esta región. En boca, buen ataque, sabor intenso, acidez bien presente remarcando las notas de espárrago.
-Ideal como aperitivo o para acompañar mariscos, ostras y frutos de frutos de mar en general.', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/vino-las-perdices-exploracion-casa-blanca-sauvignon-blanc-d_nq_np_693115-mla29480640575_022019-f1-632ae12afe7abda88f15902635029767-640-0.jpg', category: 'blancos', stock: 10},</v>
+        <v>{title: 'Las Perdices Exploracion Casablanca', price: 2150, bodega: 'Viña Las Perdices', description: 'Color verde tenue. Aromas a ruda, espárrago, hojas de tomate, con notas minerales propias de esta región. En boca, buen ataque, sabor intenso, acidez bien presente remarcando las notas de espárrago. Ideal como aperitivo o para acompañar mariscos, ostras y frutos de frutos de mar en general.', pictureUrl: 'https://d2r9epyceweg5n.cloudfront.net/stores/220/578/products/vino-las-perdices-exploracion-casa-blanca-sauvignon-blanc-d_nq_np_693115-mla29480640575_022019-f1-632ae12afe7abda88f15902635029767-640-0.jpg', category: 'blancos', stock: 10},</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>